<commit_message>
start of ACDC, but model error + not converging
</commit_message>
<xml_diff>
--- a/data/case24_ieee_rts_AC.xlsx
+++ b/data/case24_ieee_rts_AC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samho\Desktop\PhD\DC OPF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D43C68-ED88-40DC-A198-8F8FEE33A321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E947621-0E29-4218-932A-1E7B31DC94C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33480" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="11380" windowHeight="13370" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hvdc" sheetId="13" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="366">
   <si>
     <t>name</t>
   </si>
@@ -1133,16 +1133,19 @@
     <t>marginal_cost</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>MTDC</t>
+  </si>
+  <si>
     <t>Western_Link</t>
   </si>
   <si>
     <t>GB</t>
   </si>
   <si>
-    <t>Netherlands_HVDC</t>
-  </si>
-  <si>
-    <t>Non-GB</t>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -1421,13 +1424,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1745,7 +1748,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1799,7 +1802,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1838,7 +1841,7 @@
         <v>1E-4</v>
       </c>
       <c r="N2" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -1846,10 +1849,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>363</v>
-      </c>
-      <c r="B3">
-        <v>24</v>
+        <v>361</v>
+      </c>
+      <c r="B3" t="s">
+        <v>365</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -1885,7 +1888,7 @@
         <v>1E-4</v>
       </c>
       <c r="N3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="O3">
         <v>20</v>
@@ -1937,25 +1940,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="25" t="s">
         <v>348</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
     </row>
     <row r="2" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
@@ -3503,34 +3506,34 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="22">
         <v>1</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="22">
         <v>1</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="23">
         <v>1.05</v>
       </c>
-      <c r="F25" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="23" t="s">
+      <c r="F25" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="H25" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="23" t="s">
+      <c r="I25" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="25" t="s">
+      <c r="J25" s="24" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>